<commit_message>
status implementados e t1 nova
</commit_message>
<xml_diff>
--- a/saida.xlsx
+++ b/saida.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="t1.csv" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="t2.csv" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="stats" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,17 +457,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kauã Azevedo de Sousa Moreira </t>
+          <t>Ana Beatriz Cipriani Motta</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gabriel Lucas da Costa</t>
+          <t>Maria Victória Miquelito Parizani</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Karoline Horsai Manhães Saldanha</t>
+          <t>João Pedro Nogueira</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -488,71 +489,71 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lucia Nicchole Kalena de Melo Ribeiro Roque </t>
+          <t xml:space="preserve">Wallace da costa araujo </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>João Pedro Nogueira</t>
+          <t xml:space="preserve">Gabriella do Nascimento Osolins Moreira </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Geovana Rodrigues Almeida</t>
+          <t xml:space="preserve">Juliana Lopes Arcanjo </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ralf Souza Dantas da Silva</t>
+          <t>Rafael Anderson banho</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">João Victor Domingos Tavares </t>
+          <t xml:space="preserve">Kauã Azevedo de Sousa Moreira </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nathan Siqueira Muniz do Amaral</t>
+          <t xml:space="preserve">Lucia Nicchole Kalena de Melo Ribeiro Roque </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gabriella do Nascimento Osolins Moreira </t>
+          <t xml:space="preserve">Nicole Matos Alves </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Olivia Oliveira</t>
+          <t xml:space="preserve">Tais Vieira Tavares </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">José Jefferson Alves da Silva </t>
+          <t>Gabriel Leal Freitas Venancio</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Raíssa Tiezerin Costa </t>
+          <t xml:space="preserve">Maria Luiza Justino </t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Allan Douglas Vieira Santos</t>
+          <t xml:space="preserve">Georgia Miranda </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Melissa Jardim de Andrade dos Reis</t>
+          <t>Karoline Horsai Manhães Saldanha</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Gustavo Brainer</t>
+          <t xml:space="preserve">Pietra Ruas Vieira Araújo </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -564,39 +565,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ana Beatriz Cipriani Motta</t>
+          <t xml:space="preserve">Raíssa Tiezerin Costa </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kaio Nathan Carvalho Muniz Alvarenga</t>
+          <t>Gabriel Lucas da Costa</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pietra Ruas Vieira Araújo </t>
+          <t>Letícia Pinheiro Ferreira</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Maria Victória Miquelito Parizani</t>
+          <t>Gustavo Brainer</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vinícius Lima Scramignon</t>
+          <t>Maiara dos Santos da Silva</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guilherme Carvalhaes da Fonseca Ferreira </t>
+          <t>Olivia Oliveira</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Georgia Miranda </t>
+          <t xml:space="preserve">Sophia Reis </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -606,34 +607,34 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Murilo Gonçalves Barbosa </t>
+          <t xml:space="preserve">Joyce Sousa de Oliveira </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Larissa dos Santos Borges Soares</t>
+          <t xml:space="preserve">José Jefferson Alves da Silva </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Milena Gonçalves Zgerski de Carvalho</t>
+          <t xml:space="preserve">Paula Kellen Jordão Viana Manhães </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Juliana Miranda</t>
+          <t>Allan Douglas Vieira Santos</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Paula Kellen Jordão Viana Manhães </t>
+          <t xml:space="preserve">João Victor Domingos Tavares </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Juliana Lopes Arcanjo </t>
+          <t>Melissa Jardim de Andrade dos Reis</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -645,49 +646,49 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nayla Beatriz de Abreu Alves </t>
+          <t>Geovana Rodrigues Almeida</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rafaella Lima Souza da Silva</t>
+          <t>Juliana Miranda</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tais Vieira Tavares </t>
+          <t>Nathan Siqueira Muniz do Amaral</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Letícia Pinheiro Ferreira</t>
+          <t>Kaio Nathan Carvalho Muniz Alvarenga</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Maiara dos Santos da Silva</t>
+          <t>Ralf Souza Dantas da Silva</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sophia Reis </t>
+          <t>Rafaella Lima Souza da Silva</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maria Luiza Justino </t>
+          <t xml:space="preserve">Nayla Beatriz de Abreu Alves </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Victória Regina Santos Oliveira</t>
+          <t xml:space="preserve">Guilherme Carvalhaes da Fonseca Ferreira </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Gabriel Leal Freitas Venancio</t>
+          <t>Vinícius Lima Scramignon</t>
         </is>
       </c>
     </row>
@@ -699,36 +700,36 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Joyce Sousa de Oliveira </t>
+          <t>Milena Gonçalves Zgerski de Carvalho</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Rafael Lucas do Nascimento de Freitas</t>
+          <t>Rafael Louzada</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nicole Matos Alves </t>
+          <t>Victória Regina Santos Oliveira</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Rafael Anderson banho</t>
+          <t>Rafael Lucas do Nascimento de Freitas</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wallace da costa araujo </t>
+          <t xml:space="preserve">Murilo Gonçalves Barbosa </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Rafael Louzada</t>
+          <t>Larissa dos Santos Borges Soares</t>
         </is>
       </c>
     </row>
@@ -781,17 +782,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lucas Moraes Souza</t>
+          <t xml:space="preserve">Giovanna Lira Alcantara Gomes </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Matheus Dassunção</t>
+          <t>Artur Plaza</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nicolas Meirelles Pereira</t>
+          <t>Heloísa de Andrade Viveiros</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -801,68 +802,68 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Fabio Masayuki Miamoto</t>
+          <t>Jady Calil Elias Dorado</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Giovanna Lira Alcantara Gomes </t>
+          <t xml:space="preserve">Victoria Moura </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Artur Plaza</t>
+          <t>Joyce Gabriela</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Luiza Leite Carvão</t>
+          <t>Maria Luiza Dantas Pereira</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Caio Vinícius Silveira Florentino Silva </t>
+          <t xml:space="preserve">João Gabriel Pereira Costa </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guilherme Alves da Silva Ferreira </t>
+          <t>Lara Sales dos Santos</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mariana Soares de Alencar</t>
+          <t>Stefan Campaci</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Joyce Gabriela</t>
+          <t>Andrei Azevedo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Maria Luiza Dantas Pereira</t>
+          <t xml:space="preserve">Wanessa Jiaxin Su Wu </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Evely de Oliveira rodrigues </t>
+          <t>Marlon Marques Drumond</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jady Calil Elias Dorado</t>
+          <t>Leonardo Garrido de Deus</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Filipe Vieira Nascimento </t>
+          <t>Mariana Soares de Alencar</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -872,12 +873,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Davi Alves Miranda</t>
+          <t>Rodrigo José dos Santos Gonçalves</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wanessa Jiaxin Su Wu </t>
+          <t xml:space="preserve">Amanda Cristina de Castro Rocha </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -889,22 +890,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Victoria Moura </t>
+          <t>Lucas Moraes Souza</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Andrei Azevedo</t>
+          <t>Clayver Amaral</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Rodrigo José dos Santos Gonçalves</t>
+          <t xml:space="preserve">Caio Vinícius Silveira Florentino Silva </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">João Gabriel Pereira Costa </t>
+          <t>Fabio Masayuki Miamoto</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -916,51 +917,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amanda Cristina de Castro Rocha </t>
+          <t xml:space="preserve">Isabela Sousa Silva </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Clayver Amaral</t>
+          <t>Matheus Dassunção</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Guilherme Nabuco da Fonseca</t>
+          <t>sofia fagundes monteiro de melo gomes</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guilherme Alves da Silva Ferreira </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pedro Henrique Souza de Castro </t>
+          <t xml:space="preserve">Evely de Oliveira rodrigues </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Isabela Sousa Silva </t>
+          <t>Ygor Matheus Silva do Amaral</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Heloísa de Andrade Viveiros</t>
+          <t>Nicolas Meirelles Pereira</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Marlon Marques Drumond</t>
+          <t xml:space="preserve">Matheus Alexssander Fontoura Vieira Silveira </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Filipe Vieira Nascimento </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Leonardo Garrido de Deus</t>
+          <t xml:space="preserve">Vinícius Sá Silva </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Eliza de Oliveira Pinto Paulino</t>
+          <t>Davi Alves Miranda</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -970,46 +981,36 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Luiza Leite Carvão</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Francisco Jailson da Silva Vicente </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
           <t xml:space="preserve">Vitor Henrique de Castro Gabriel </t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pedro Henrique Souza de Castro </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mariana Rios de Andrade</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Maria Rosa Paes</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Ygor Matheus Silva do Amaral</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Stefan Campaci</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Vinícius Sá Silva </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Lara Sales dos Santos</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Tiago Mendes Correa</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Francisco Jailson da Silva Vicente </t>
         </is>
       </c>
     </row>
@@ -1021,20 +1022,111 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Mariana Rios de Andrade</t>
+          <t>Tiago Mendes Correa</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>sofia fagundes monteiro de melo gomes</t>
+          <t>Guilherme Nabuco da Fonseca</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Matheus Alexssander Fontoura Vieira Silveira </t>
-        </is>
+          <t>Eliza de Oliveira Pinto Paulino</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Prioridades/Repetições</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>t1.csv</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>t2.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>